<commit_message>
more result int result2
</commit_message>
<xml_diff>
--- a/result2.xlsx
+++ b/result2.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="22">
   <si>
     <t>anti_2</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -118,7 +118,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -158,6 +158,14 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -181,7 +189,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -196,6 +204,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -480,13 +491,17 @@
   <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.15">
@@ -632,15 +647,21 @@
         <v>9798</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="F4" s="1">
+        <v>2862</v>
+      </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
+      <c r="J4" s="1">
+        <v>3199</v>
+      </c>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
+      <c r="N4" s="1">
+        <v>1361</v>
+      </c>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
@@ -710,6 +731,15 @@
       </c>
       <c r="D6" s="1">
         <v>16124719</v>
+      </c>
+      <c r="F6" s="1">
+        <v>40136320</v>
+      </c>
+      <c r="J6" s="1">
+        <v>44043805</v>
+      </c>
+      <c r="N6" s="1">
+        <v>14458753</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.15">
@@ -1129,7 +1159,9 @@
       <c r="G16" s="1">
         <v>347</v>
       </c>
-      <c r="H16" s="2"/>
+      <c r="H16" s="1">
+        <v>52884</v>
+      </c>
       <c r="I16" s="3"/>
       <c r="J16" s="1">
         <v>85</v>
@@ -1168,8 +1200,8 @@
       <c r="G17" s="1">
         <v>458</v>
       </c>
-      <c r="H17" s="3" t="s">
-        <v>16</v>
+      <c r="H17" s="5">
+        <v>14105</v>
       </c>
       <c r="I17" s="3" t="s">
         <v>11</v>
@@ -1220,6 +1252,9 @@
       </c>
       <c r="G18" s="1">
         <v>852147</v>
+      </c>
+      <c r="H18" s="1">
+        <v>36861622</v>
       </c>
       <c r="J18" s="1">
         <v>392941</v>

</xml_diff>